<commit_message>
Upgrade: -Cambio Index da vin a targa; -Cambio numero minimo di posti
</commit_message>
<xml_diff>
--- a/DB-FIRST.xlsx
+++ b/DB-FIRST.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>TABELLA AUTO</t>
   </si>
@@ -79,18 +79,15 @@
     <t>NOT NULL, UNIQUE</t>
   </si>
   <si>
+    <t>INDEX</t>
+  </si>
+  <si>
     <t>numero_telaio</t>
   </si>
   <si>
     <t>VARCHAR(17)</t>
   </si>
   <si>
-    <t>NOT NULL,UNIQUE</t>
-  </si>
-  <si>
-    <t>INDEX</t>
-  </si>
-  <si>
     <t>anno_produzione</t>
   </si>
   <si>
@@ -121,7 +118,7 @@
     <t>numero_occupanti</t>
   </si>
   <si>
-    <t>NOT NULL, DEFAULT (1)</t>
+    <t>NOT NULL, DEFAULT (2)</t>
   </si>
   <si>
     <t>revisione</t>
@@ -629,28 +626,28 @@
       <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>25</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12">
       <c r="B12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>11</v>
@@ -659,7 +656,7 @@
     </row>
     <row r="13">
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
@@ -671,7 +668,7 @@
     </row>
     <row r="14">
       <c r="B14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>15</v>
@@ -683,10 +680,10 @@
     </row>
     <row r="15">
       <c r="B15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>11</v>
@@ -695,10 +692,10 @@
     </row>
     <row r="16">
       <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>11</v>
@@ -707,7 +704,7 @@
     </row>
     <row r="17">
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>6</v>
@@ -719,19 +716,19 @@
     </row>
     <row r="18">
       <c r="B18" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="7"/>
     </row>
     <row r="19">
       <c r="B19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>15</v>
@@ -743,7 +740,7 @@
     </row>
     <row r="22">
       <c r="B22" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3"/>
     </row>
@@ -759,10 +756,10 @@
     </row>
     <row r="25">
       <c r="B25" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="26">
@@ -770,7 +767,7 @@
         <v>1.0</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27">
@@ -778,7 +775,7 @@
         <v>2.0</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28">
@@ -786,7 +783,7 @@
         <v>3.0</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29">
@@ -794,7 +791,7 @@
         <v>4.0</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30">
@@ -803,16 +800,16 @@
     </row>
     <row r="31">
       <c r="B31" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="3"/>
     </row>
     <row r="32">
       <c r="B32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="33">
@@ -820,7 +817,7 @@
         <v>1.0</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34">
@@ -828,7 +825,7 @@
         <v>2.0</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35">
@@ -836,7 +833,7 @@
         <v>3.0</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36">
@@ -844,7 +841,7 @@
         <v>4.0</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37">
@@ -852,7 +849,7 @@
         <v>5.0</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38">
@@ -860,7 +857,7 @@
         <v>6.0</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39">
@@ -869,7 +866,7 @@
     </row>
     <row r="40">
       <c r="B40" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" s="3"/>
     </row>
@@ -878,7 +875,7 @@
         <v>1.0</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42">
@@ -886,16 +883,16 @@
         <v>2.0</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>